<commit_message>
working with xarrays to rebuild model
</commit_message>
<xml_diff>
--- a/Data/Indices/County_names.xlsx
+++ b/Data/Indices/County_names.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://caenergy-my.sharepoint.com/personal/alan_jian_energy_ca_gov/Documents/work/Projects/Analytica Replace/MDHD Model Conversion/Indices/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://caenergy-my.sharepoint.com/personal/alan_jian_energy_ca_gov/Documents/work/Projects/Analytica Replace/MDHD Model Conversion/Python _i23 Freight Model/Data/Indices/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_F25DC773A252ABDACC1048E7A11B74EC5BDE58F2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7A047AF-477B-435B-B6CE-C8286CBC17FD}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="11_F25DC773A252ABDACC1048E7A11B74EC5BDE58F2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A8AEAA6-EE3A-4DE6-9F3F-600FBBAEE232}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="2685" windowWidth="28800" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="28800" windowHeight="11325" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Counties" sheetId="1" r:id="rId1"/>
+    <sheet name="README" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Alameda</t>
   </si>
@@ -199,14 +200,52 @@
   </si>
   <si>
     <t>Yuba</t>
+  </si>
+  <si>
+    <t>Counties</t>
+  </si>
+  <si>
+    <r>
+      <t>IEPR:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2024</t>
+    </r>
+  </si>
+  <si>
+    <t>Description:</t>
+  </si>
+  <si>
+    <t>Usage:</t>
+  </si>
+  <si>
+    <t>This describes the county level labels used in our data.</t>
+  </si>
+  <si>
+    <t>Double check any county-level data going into the model to make sure they match these labels.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -234,8 +273,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,302 +556,347 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A58"/>
+  <dimension ref="A1:A59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
+      <c r="A1" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27BC23D0-1B3B-4A27-843F-1C1B5309FFB9}">
+  <dimension ref="A2:A8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>